<commit_message>
updated upgrade on 02/06/2020
</commit_message>
<xml_diff>
--- a/Excel/searchnep.xlsx
+++ b/Excel/searchnep.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61F4A90-A69E-45D2-8005-BDBF8D5880A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A63D33D-B61C-4B96-B770-3BF3A9F7F1A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3495" yWindow="2280" windowWidth="15375" windowHeight="7890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3735" yWindow="3495" windowWidth="15375" windowHeight="7890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Authenticate" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="117">
   <si>
     <t>Marital status</t>
   </si>
@@ -353,6 +353,21 @@
   </si>
   <si>
     <t>https://www.iyermatrimony.com/</t>
+  </si>
+  <si>
+    <t>Payment Code</t>
+  </si>
+  <si>
+    <t>&amp;countryCode=149</t>
+  </si>
+  <si>
+    <t>&amp;countryCode=222</t>
+  </si>
+  <si>
+    <t>&amp;countryCode=195</t>
+  </si>
+  <si>
+    <t>&amp;countryCode=18</t>
   </si>
 </sst>
 </file>
@@ -747,19 +762,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -772,8 +788,11 @@
       <c r="D1" t="s">
         <v>99</v>
       </c>
+      <c r="E1" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -786,8 +805,11 @@
       <c r="D2" s="3" t="s">
         <v>101</v>
       </c>
+      <c r="E2" t="s">
+        <v>113</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>89</v>
       </c>
@@ -800,8 +822,11 @@
       <c r="D3" s="3" t="s">
         <v>100</v>
       </c>
+      <c r="E3" t="s">
+        <v>114</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -814,8 +839,11 @@
       <c r="D4" s="3" t="s">
         <v>102</v>
       </c>
+      <c r="E4" t="s">
+        <v>115</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>109</v>
       </c>
@@ -827,6 +855,9 @@
       </c>
       <c r="D5" s="3" t="s">
         <v>111</v>
+      </c>
+      <c r="E5" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>